<commit_message>
Adds more reading of things
</commit_message>
<xml_diff>
--- a/carl_test.xlsx
+++ b/carl_test.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fractal ERA\Desktop\Examensarbete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6992F0-6259-4CDF-AC3C-754F910BE12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF67A91-C9C0-4811-8AC3-9F397318CABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20220" yWindow="2580" windowWidth="16560" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1215" windowWidth="20505" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Leadership" sheetId="1" r:id="rId1"/>
+    <sheet name="Personal" sheetId="2" r:id="rId2"/>
+    <sheet name="Social" sheetId="3" r:id="rId3"/>
+    <sheet name="Intellectual" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Yrkestitel</t>
   </si>
@@ -90,16 +93,93 @@
   </si>
   <si>
     <t>Tolk</t>
+  </si>
+  <si>
+    <t>PERSONAL1</t>
+  </si>
+  <si>
+    <t>PERSONAL2</t>
+  </si>
+  <si>
+    <t>PERSONAL3</t>
+  </si>
+  <si>
+    <t>PERONSLA4</t>
+  </si>
+  <si>
+    <t>PERSONAL5</t>
+  </si>
+  <si>
+    <t>PERSONAL7</t>
+  </si>
+  <si>
+    <t>PERERASD</t>
+  </si>
+  <si>
+    <t>SOCIAL2</t>
+  </si>
+  <si>
+    <t>SOCIAL4</t>
+  </si>
+  <si>
+    <t>SOCIAL5</t>
+  </si>
+  <si>
+    <t>SOCIAL3</t>
+  </si>
+  <si>
+    <t>SOCIAL6</t>
+  </si>
+  <si>
+    <t>SOCIAL7</t>
+  </si>
+  <si>
+    <t>SOCIAL1</t>
+  </si>
+  <si>
+    <t>INT1</t>
+  </si>
+  <si>
+    <t>INT2</t>
+  </si>
+  <si>
+    <t>INT3</t>
+  </si>
+  <si>
+    <t>INT4</t>
+  </si>
+  <si>
+    <t>INT5</t>
+  </si>
+  <si>
+    <t>INT6</t>
+  </si>
+  <si>
+    <t>INT7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,16 +208,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,4 +809,442 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9B9CB5-B706-4240-BE21-E0C54A7DF26E}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>56</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>55</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>55</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D7E778-DB4A-4EA7-B862-AE8084A2141A}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>56</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>55</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>55</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A1DE3B-1921-4B1B-9208-972A430C2AAF}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>56</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>55</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>55</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1" display="Socialö@" xr:uid="{4E83A5A9-94DA-4C73-971A-CE6C31EBB994}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update raw training data
</commit_message>
<xml_diff>
--- a/carl_test.xlsx
+++ b/carl_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fractal ERA\Desktop\Examensarbete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF67A91-C9C0-4811-8AC3-9F397318CABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A972F43F-5D9C-4D58-A151-4ED4009BCF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1215" windowWidth="20505" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23625" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leadership" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Yrkestitel</t>
   </si>
@@ -95,85 +95,95 @@
     <t>Tolk</t>
   </si>
   <si>
-    <t>PERSONAL1</t>
-  </si>
-  <si>
-    <t>PERSONAL2</t>
-  </si>
-  <si>
-    <t>PERSONAL3</t>
-  </si>
-  <si>
-    <t>PERONSLA4</t>
-  </si>
-  <si>
-    <t>PERSONAL5</t>
-  </si>
-  <si>
-    <t>PERSONAL7</t>
-  </si>
-  <si>
-    <t>PERERASD</t>
-  </si>
-  <si>
-    <t>SOCIAL2</t>
-  </si>
-  <si>
-    <t>SOCIAL4</t>
-  </si>
-  <si>
-    <t>SOCIAL5</t>
-  </si>
-  <si>
-    <t>SOCIAL3</t>
-  </si>
-  <si>
-    <t>SOCIAL6</t>
-  </si>
-  <si>
-    <t>SOCIAL7</t>
-  </si>
-  <si>
-    <t>SOCIAL1</t>
-  </si>
-  <si>
-    <t>INT1</t>
-  </si>
-  <si>
-    <t>INT2</t>
-  </si>
-  <si>
-    <t>INT3</t>
-  </si>
-  <si>
-    <t>INT4</t>
-  </si>
-  <si>
-    <t>INT5</t>
-  </si>
-  <si>
-    <t>INT6</t>
-  </si>
-  <si>
-    <t>INT7</t>
+    <t>PERSONLIG MOGNAD</t>
+  </si>
+  <si>
+    <t>INTEGRITET</t>
+  </si>
+  <si>
+    <t>SJÄLVSTÄNDIGHET</t>
+  </si>
+  <si>
+    <t>INITIATIVTAGANDE</t>
+  </si>
+  <si>
+    <t>SJÄLVGÅENDE</t>
+  </si>
+  <si>
+    <t>FLEXIBEL</t>
+  </si>
+  <si>
+    <t>STABIL</t>
+  </si>
+  <si>
+    <t>PRESTATIONSORIENTERAD</t>
+  </si>
+  <si>
+    <t>ENERGISK</t>
+  </si>
+  <si>
+    <t>UTHÅLLIG</t>
+  </si>
+  <si>
+    <t>MÅL OCH RESULTATORIENTERAD</t>
+  </si>
+  <si>
+    <t>SAMARBETSFÖRMÅGA</t>
+  </si>
+  <si>
+    <t>RELATIONSSKAPANDE</t>
+  </si>
+  <si>
+    <t>EMPATISK FÖRMÅGA</t>
+  </si>
+  <si>
+    <t>MUNTLIG KOMMUNIKATION</t>
+  </si>
+  <si>
+    <t>LOJAL</t>
+  </si>
+  <si>
+    <t>SERVICEINRIKTAD</t>
+  </si>
+  <si>
+    <t>ÖVERTYGANDE</t>
+  </si>
+  <si>
+    <t>KULTURELL MEDVETENHET</t>
+  </si>
+  <si>
+    <t>PEDAGOGISK INSIKT</t>
+  </si>
+  <si>
+    <t>STRUKTURERAD</t>
+  </si>
+  <si>
+    <t>KVALITETSMEDVETEN</t>
+  </si>
+  <si>
+    <t>KREATIV</t>
+  </si>
+  <si>
+    <t>SPECIALISTKUNSKAP</t>
+  </si>
+  <si>
+    <t>PROBLEMLÖSANDE ANALYSFÖRMÅGA</t>
+  </si>
+  <si>
+    <t>NUMERISK ANALYTISK FÖRMÅGA</t>
+  </si>
+  <si>
+    <t>SPRÅKLIG ANALYTISK FÖRMÅGA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +205,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -208,22 +236,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,67 +845,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9B9CB5-B706-4240-BE21-E0C54A7DF26E}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -881,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -890,16 +960,28 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -907,7 +989,7 @@
         <v>30</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -916,39 +998,291 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>35</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>22</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>9</v>
+      </c>
+      <c r="L8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>30</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -958,101 +1292,131 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D7E778-DB4A-4EA7-B862-AE8084A2141A}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F2">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F3">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1061,21 +1425,27 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G4">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1084,16 +1454,214 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="G5">
         <v>30</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>45</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1103,148 +1671,315 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A1DE3B-1921-4B1B-9208-972A430C2AAF}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
-        <v>1</v>
+      <c r="E2" s="2">
+        <v>42</v>
       </c>
       <c r="F2">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>55</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
+      <c r="H9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11" si="0">SUM(B11:H11)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" display="Socialö@" xr:uid="{4E83A5A9-94DA-4C73-971A-CE6C31EBB994}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>